<commit_message>
updated the jupyter cell and border color
</commit_message>
<xml_diff>
--- a/colors.xlsx
+++ b/colors.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/mohammadfarshchin/Desktop/julia-light-theme/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/mohammadfarshchin/Desktop/vscode-julia-theme/julia-light/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1D208C01-7A3D-5C44-9817-F31E922F60D9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{83C44113-20AD-8942-8D48-E471FE861DE7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="33300" yWindow="-1960" windowWidth="19240" windowHeight="14900" xr2:uid="{D40CDA91-5177-A14A-B377-F3F7BAD328E2}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="12">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="13">
   <si>
     <t>Comments</t>
   </si>
@@ -70,13 +70,16 @@
   </si>
   <si>
     <t>numeric</t>
+  </si>
+  <si>
+    <t>cell color</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -96,8 +99,15 @@
       <name val="Menlo"/>
       <family val="2"/>
     </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FFF5F5F5"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="12">
+  <fills count="13">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -161,6 +171,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FF408080"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF5F5F5"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -177,7 +193,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="14">
+  <cellXfs count="15">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -216,6 +232,9 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="11" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="12" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -226,6 +245,8 @@
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <colors>
     <mruColors>
+      <color rgb="FFF5F5F5"/>
+      <color rgb="FFBDBDBD"/>
       <color rgb="FF408080"/>
       <color rgb="FF008801"/>
       <color rgb="FF1F8A22"/>
@@ -234,8 +255,6 @@
       <color rgb="FFAA23FF"/>
       <color rgb="FF008000"/>
       <color rgb="FFBA2121"/>
-      <color rgb="FF2A00FF"/>
-      <color rgb="FF007B00"/>
     </mruColors>
   </colors>
   <extLst>
@@ -546,10 +565,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{951F14BF-13C0-1644-8D33-63FCA456CC3C}">
-  <dimension ref="A1:C12"/>
+  <dimension ref="A1:C13"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H5" sqref="H5"/>
+    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="D14" sqref="D14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="43" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -635,6 +654,12 @@
         <v>11</v>
       </c>
     </row>
+    <row r="13" spans="1:3" ht="43" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A13" s="14"/>
+      <c r="B13" s="1" t="s">
+        <v>12</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>